<commit_message>
changes in network project add a new monthly section in claim and in attendnce  and correct the sidebar view monthly p&l section and correct the circle show uniqe in busniess section
</commit_message>
<xml_diff>
--- a/public/uploads/excel/5af04bf4be2d4570b2a25735.xlsx
+++ b/public/uploads/excel/5af04bf4be2d4570b2a25735.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Input" r:id="rId4"/>
+    <sheet sheetId="1" name="Input" state="show" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -56,60 +56,6 @@
   </si>
   <si>
     <t>Invoice_Status</t>
-  </si>
-  <si>
-    <t>HWMP</t>
-  </si>
-  <si>
-    <t>Huawei</t>
-  </si>
-  <si>
-    <t>4G-SCFT</t>
-  </si>
-  <si>
-    <t>1121_TDD13</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>1121_TDD13-8.3:Single site verification without tools (LTE)-4G-SCFT</t>
-  </si>
-  <si>
-    <t>A14</t>
-  </si>
-  <si>
-    <t>A14-8.3:Single site verification without tools (LTE)-4G-SCFT</t>
-  </si>
-  <si>
-    <t>SMDL</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>TDD_NBD004</t>
-  </si>
-  <si>
-    <t>TDD_NBD004-8.3:Single site verification without tools (LTE)-4G-SCFT</t>
-  </si>
-  <si>
-    <t>TDD_JAI207</t>
-  </si>
-  <si>
-    <t>TDD_JAI207-8.3:Single site verification without tools (LTE)-4G-SCFT</t>
-  </si>
-  <si>
-    <t>TDD_DHO011</t>
-  </si>
-  <si>
-    <t>TDD_DHO011-8.3:Single site verification without tools (LTE)-4G-SCFT</t>
-  </si>
-  <si>
-    <t>TDD_HTNI01</t>
-  </si>
-  <si>
-    <t>TDD_HTNI01-8.3:Single site verification without tools (LTE)-4G-SCFT</t>
   </si>
 </sst>
 </file>
@@ -486,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="10" customWidth="1"/>
@@ -541,162 +487,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2">
-        <v>6001</v>
-      </c>
-      <c r="H2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3">
-        <v>6003</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4">
-        <v>4370</v>
-      </c>
-      <c r="H4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5">
-        <v>4370</v>
-      </c>
-      <c r="H5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6">
-        <v>4370</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7">
-        <v>4370</v>
-      </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>